<commit_message>
Novos gráficos - WID
</commit_message>
<xml_diff>
--- a/tables/resultados_distributivos_com_arrecadacao.xlsx
+++ b/tables/resultados_distributivos_com_arrecadacao.xlsx
@@ -407,10 +407,10 @@
         <v>0.1408914272615971</v>
       </c>
       <c r="D2">
-        <v>0.5660957309895703</v>
+        <v>0.5489325840217185</v>
       </c>
       <c r="E2">
-        <v>0.3163143350756296</v>
+        <v>0.2484647400409127</v>
       </c>
       <c r="F2">
         <v>370.9051059178454</v>
@@ -432,10 +432,10 @@
         <v>0.1408192576692769</v>
       </c>
       <c r="D3">
-        <v>0.5640953737327782</v>
+        <v>0.5462247212009397</v>
       </c>
       <c r="E3">
-        <v>0.3098311902079652</v>
+        <v>0.2420163501452704</v>
       </c>
       <c r="F3">
         <v>367.565927956492</v>
@@ -457,10 +457,10 @@
         <v>0.1413610485529083</v>
       </c>
       <c r="D4">
-        <v>0.5624182653844367</v>
+        <v>0.5444788569396176</v>
       </c>
       <c r="E4">
-        <v>0.3071758206548156</v>
+        <v>0.2390291355613186</v>
       </c>
       <c r="F4">
         <v>392.3839477842254</v>

</xml_diff>